<commit_message>
:sparkles: feat: Adicionando fórmulas na planilha
</commit_message>
<xml_diff>
--- a/data/bar_chart.xlsx
+++ b/data/bar_chart.xlsx
@@ -16,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +29,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,17 +61,20 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -138,7 +150,6 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -679,7 +690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,6 +826,36 @@
         <v>588500</v>
       </c>
     </row>
+    <row r="6">
+      <c r="B6" s="2">
+        <f>SUM(B2:B5)</f>
+        <v/>
+      </c>
+      <c r="C6" s="2">
+        <f>SUM(C2:C5)</f>
+        <v/>
+      </c>
+      <c r="D6" s="2">
+        <f>SUM(D2:D5)</f>
+        <v/>
+      </c>
+      <c r="E6" s="2">
+        <f>SUM(E2:E5)</f>
+        <v/>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(F2:F5)</f>
+        <v/>
+      </c>
+      <c r="G6" s="2">
+        <f>SUM(G2:G5)</f>
+        <v/>
+      </c>
+      <c r="H6" s="2">
+        <f>SUM(H2:H5)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>